<commit_message>
Atualização documentação conferência LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CAP.xlsx
+++ b/Documentação/Planilhas/Conferencia_CAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="stg_cap_titulo_referencia" sheetId="94" r:id="rId3"/>
     <sheet name="stg_cap_titulo" sheetId="95" r:id="rId4"/>
     <sheet name="stg_cap_reembolso" sheetId="96" r:id="rId5"/>
+    <sheet name="stg_cap_titulo_pgto" sheetId="98" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="476">
   <si>
     <t>1</t>
   </si>
@@ -534,13 +535,6 @@
   </si>
   <si>
     <t>Conferência dos dados da tabela:</t>
-  </si>
-  <si>
-    <t>Sessão tfacp2520m000 [no menu Exibições, selecionar "Incluindo Faturas Totalmente Pagas"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sessão tfacp2523m000 
-[selecionar o título desejado na sessão tfacp2520m000 e escolher no menu Referências a opção "Documentos relacionados ao pagamento por entrada aberta"] </t>
   </si>
   <si>
     <t>Pegar a terceira informação da coluna Docum.</t>
@@ -588,12 +582,6 @@
     <t>Pegar a informação da coluna Valor da Transação</t>
   </si>
   <si>
-    <t>sessão tfacp2524s000 [selecionar o Documento na sessão tfacp2523m000  e escolher Referências, Detalhes</t>
-  </si>
-  <si>
-    <t>No cabeçalho da tela, linha Documento de Pagamento, possui 4 colunas de informação. Pegar as duas últimas colunas.</t>
-  </si>
-  <si>
     <t>tfacp2520m000, tfacp2523m000, tfacp2524s000</t>
   </si>
   <si>
@@ -603,14 +591,6 @@
     <t>Gerado a partir do CD_TRANSACAO_DOCUMENTO.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'PLG' = 1
- 'LKF' = 2
- 'PKF' = 2
-  'RKF'= 4
-Se a categoria retornar 10 de acordo com o CD_TRANSACAO_DOCUMENTO = 3
-Caso contrário = 0</t>
-  </si>
-  <si>
     <t>Regra utilizada:</t>
   </si>
   <si>
@@ -797,12 +777,6 @@
     <t>sessão tdrecl547m50l</t>
   </si>
   <si>
-    <t>sessão tdrecl505m50l [selecionar a referência fiscal na sessão tdrecl547m50l e no menu Ações, selecionar Linhas Rec Fiscal - Sumário</t>
-  </si>
-  <si>
-    <t>Pegar a informação da coluna Valor da Mercadoria [se tiver mais de um valor será necessário somá-los]</t>
-  </si>
-  <si>
     <t>dbo.stg_cap_titulo</t>
   </si>
   <si>
@@ -1106,12 +1080,6 @@
     <t>Fixo CAP</t>
   </si>
   <si>
-    <t>Pegar a segunda infromação da coluna Docum.</t>
-  </si>
-  <si>
-    <t>Pegar a primeira infromação da coluna Docum.</t>
-  </si>
-  <si>
     <t>Se  CD_TRANSACAO_TITULO for  'AGA' ou 'GA1', retornará 3. Caso contrário, 2.</t>
   </si>
   <si>
@@ -1131,12 +1099,6 @@
   </si>
   <si>
     <t>Pegar a informação da coluna Data do Vencimento</t>
-  </si>
-  <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências, Progr. Pagamento. Pegar a informação da coluna Data Vencimento Original</t>
-  </si>
-  <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências, Documentos Relacionados ao Pagamento por Entrada em Aberto. Selecionar a linha cujo tipo de documento seja igual à Pagamento Normal e no menu Referências, escolher a opção Documentos da Fatura por Pagamento. No cabeçalho, pegar a informação da Data do Pagamento</t>
   </si>
   <si>
     <t>Pegar a informação da coluna Valor</t>
@@ -1150,9 +1112,6 @@
   <si>
     <t>Pedir o detalhamento da linha selecionada. No cabeçalho da tela, pegar a informação do Aprovado para pagamento.
 Se estiver com Não ou Não aplicável será 2. Se tiver como sim, será 1</t>
-  </si>
-  <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências, Progr. Pagamento. Pegar a informação da coluna Status do Pagamento</t>
   </si>
   <si>
     <t xml:space="preserve">1-Não aplicável
@@ -1192,9 +1151,6 @@
     <t>Pegar informação da coluna Valor do Saldo [BRL]</t>
   </si>
   <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências, Progr. Pagamento e na sequência, detalhar a linha apresentada. Na aba Geral, pegar a primeira informação apresentada no campo Banco do Fornecedor</t>
-  </si>
-  <si>
     <t>Fazer a seleção do CD_BANCO_DESTINO no campo Banco Oficial. Pegar a informação da coluna Agência</t>
   </si>
   <si>
@@ -1205,13 +1161,6 @@
   </si>
   <si>
     <t>Fazer a seleção do CD_BANCO_DESTINO no campo Banco e pedir o seu detalhamento.  Na aba Detalhes,  seção Detalhes do Banco Pegar a segunda informação do campo Conta Bancária</t>
-  </si>
-  <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências,Documentos relacionados ao pagamento por entrada aberto. Selecionar a linha apresentada e no menu Referências, pedir Detalhes.
-Na aba Valor, pegar a informação de Multa por atraso de Pagamento</t>
-  </si>
-  <si>
-    <t>Com o botão direito do mouse sobre a linha desejada, escolher Referências, Progr. Pagamento. Pegar a informação da coluna Valor Taxa/Juros</t>
   </si>
   <si>
     <t>Segundo o Fábio da INFOR, essa informação não virá nesta base, pois aqui só conseguimos tratar os dados de Atacado e Varejo</t>
@@ -1357,6 +1306,193 @@
 Nr Pedido Loja = Nr Ped Cliente a ser dev ou trocado
 Nr Entrega = Nr Entrega a ser dev ou trocada
 Sequencial = Sequencial item a ser dev ou trocado</t>
+  </si>
+  <si>
+    <t>dbo.stg_cap_titulo_pgto</t>
+  </si>
+  <si>
+    <t>CD_BANCO</t>
+  </si>
+  <si>
+    <t>NR_AGENCIA</t>
+  </si>
+  <si>
+    <t>NR_CONTA_CORRENTE</t>
+  </si>
+  <si>
+    <t>CD_MODALIDADE_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>SQ_DOCUMENTO</t>
+  </si>
+  <si>
+    <t>DT_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>VL_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>DT_ESTORNO</t>
+  </si>
+  <si>
+    <t>CD_SITUACAO_PAGTO_ELETRONICO</t>
+  </si>
+  <si>
+    <t>CD_SITUACAO_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>CD_METODO_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>PAE</t>
+  </si>
+  <si>
+    <t>388000.0000</t>
+  </si>
+  <si>
+    <t>2014-07-01 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2120</t>
+  </si>
+  <si>
+    <t>000000038</t>
+  </si>
+  <si>
+    <t>BOP</t>
+  </si>
+  <si>
+    <t>12000.0000</t>
+  </si>
+  <si>
+    <t>000000193</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2014-06-10 11:58:51.000</t>
+  </si>
+  <si>
+    <t>PAG2</t>
+  </si>
+  <si>
+    <t>156456</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>2014-06-10 12:46:15.000</t>
+  </si>
+  <si>
+    <t>37000.0000</t>
+  </si>
+  <si>
+    <t>PBG2</t>
+  </si>
+  <si>
+    <t>2014-03-06 11:37:13.000</t>
+  </si>
+  <si>
+    <t>409200.0000</t>
+  </si>
+  <si>
+    <t>2014-03-06 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2014-06-25 00:00:00.000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2014-05-19 10:53:10.000</t>
+  </si>
+  <si>
+    <t>2000.0000</t>
+  </si>
+  <si>
+    <t>2014-05-19 00:00:00.000</t>
+  </si>
+  <si>
+    <t>PFS2</t>
+  </si>
+  <si>
+    <t>000000271</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>2014-06-05 16:49:40.000</t>
+  </si>
+  <si>
+    <t>25000.0000</t>
+  </si>
+  <si>
+    <t>2014-06-05 00:00:00.000</t>
+  </si>
+  <si>
+    <t>PKK2</t>
+  </si>
+  <si>
+    <t>1024</t>
+  </si>
+  <si>
+    <t>Sessão tfacp2520m000 [no menu Specific, selecionar "Incluindo Faturas Totalmente Pagas"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sessão tfacp2523m000 
+[selecionar o título desejado na sessão tfacp2520m000 e com o botão direito do mouse escolher Specific ==&gt; "Documentos relacionados ao pagamento por entrada aberta"] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PLG' = 1
+ 'LKF' = 2
+ 'PKF' = 2
+  'RKF'= 4
+Se a categoria retornar 10 de acordo com o CD_TRANSACAO_DOCUMENTO, então virá 3
+Caso contrário = 0</t>
+  </si>
+  <si>
+    <t>sessão tfacp2524s000 [selecionar o Documento na sessão tfacp2523m000  e escolher Specific, Detalhes</t>
+  </si>
+  <si>
+    <t>No cabeçalho da tela , a linha Documento de Pagamento, possui 4 colunas de informação. Pegar as duas últimas colunas.</t>
+  </si>
+  <si>
+    <t>sessão tdrecl505m50l [selecionar a referência fiscal na sessão tdrecl547m50l e no menu Specific, selecionar Linhas Rec Fiscal - Sumário</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna Valor da Mercadoria [se tiver mais de um item vendido, será necessário somá-los]</t>
+  </si>
+  <si>
+    <t>No menu Specific, selecionar "Incluindo Faturas Totalmente Pagas"</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific, Progr. Pagamento. Pegar a informação da coluna Data Vencimento Original</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific, Documentos Relacionados ao Pagamento por Entrada em Aberto. Selecionar a linha cujo tipo de documento seja igual à Pagamento Normal e no menu Specific, escolher a opção Documentos da Fatura por Pagamento. No cabeçalho, pegar a informação da Data do Pagamento</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific, Progr. Pagamento. Pegar a informação da coluna Status do Pagamento</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific,Documentos relacionados ao pagamento por entrada aberto. Selecionar a linha apresentada e no menu Specific, pedir Detalhes.
+Na aba Valor, pegar a informação de Multa por atraso de Pagamento</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific, Progr. Pagamento e na sequência, detalhar a linha apresentada. Na aba Geral, pegar a primeira informação apresentada no campo Banco do Fornecedor</t>
+  </si>
+  <si>
+    <t>Com o botão direito do mouse sobre a linha desejada, escolher Specific, Progr. Pagamento. Pegar a informação da coluna Valor Juros</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1857,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1785,6 +1921,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1839,18 +1981,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1860,6 +1990,21 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1868,19 +2013,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1901,6 +2033,51 @@
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3324225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21659850" y="4286250"/>
+          <a:ext cx="3152775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2736,8 +2913,8 @@
   </sheetPr>
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView topLeftCell="Q7" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23:R25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2768,10 +2945,10 @@
       <c r="AD1" s="2"/>
     </row>
     <row r="2" spans="1:30" ht="21">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
         <v>164</v>
       </c>
@@ -2779,25 +2956,25 @@
       <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30" ht="21">
-      <c r="A3" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="43"/>
+      <c r="A3" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="45"/>
       <c r="C3" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="S3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" ht="21">
-      <c r="A4" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="1"/>
       <c r="O4" s="14"/>
       <c r="S4" s="2"/>
@@ -3428,178 +3605,178 @@
     <row r="20" spans="1:18" ht="11.25" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
-      <c r="D20" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q20" s="33" t="s">
-        <v>192</v>
+      <c r="D20" s="36" t="s">
+        <v>462</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="36" t="s">
+        <v>463</v>
+      </c>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q20" s="35" t="s">
+        <v>187</v>
       </c>
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="11.25" customHeight="1">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="33"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="35"/>
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" ht="11.25" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="33"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="35"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="J23" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="K23" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="J23" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="L23" s="29" t="s">
+      <c r="L23" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="M23" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="N23" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="M23" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="N23" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="O23" s="29" t="s">
+      <c r="O23" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="P23" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q23" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="P23" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q23" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="R23" s="32" t="s">
-        <v>191</v>
+      <c r="R23" s="34" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="32"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="34"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="32"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="34"/>
     </row>
     <row r="27" spans="1:18">
       <c r="K27" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="247.5">
       <c r="K28" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>189</v>
+        <v>464</v>
       </c>
       <c r="P28" s="24"/>
       <c r="Q28" s="22"/>
@@ -3635,6 +3812,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3646,7 +3824,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="A29:D29"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3663,267 +3841,267 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="21">
+      <c r="A3" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="21">
-      <c r="A3" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="11.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="29" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" ht="11.25" customHeight="1">
+      <c r="A22" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="D22" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="27" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="27"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="27"/>
-    </row>
-    <row r="22" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A22" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>253</v>
+      <c r="E22" s="31" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3949,8 +4127,8 @@
   </sheetPr>
   <dimension ref="A2:AH30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="Y4" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23:AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3967,7 +4145,7 @@
     <col min="10" max="10" width="21.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="39.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="2" customWidth="1"/>
     <col min="14" max="14" width="28.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="38.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" style="2" customWidth="1"/>
@@ -3992,32 +4170,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="21">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="21">
-      <c r="A3" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="43"/>
+      <c r="A3" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="45"/>
       <c r="C3" s="3" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="21">
-      <c r="A4" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="1"/>
       <c r="O4" s="14"/>
       <c r="P4" s="1"/>
@@ -4052,88 +4230,88 @@
         <v>94</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD7" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="AC7" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="AE7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AF7" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="AG7" s="6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:33" s="5" customFormat="1">
@@ -4159,37 +4337,37 @@
         <v>0</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>109</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>1</v>
@@ -4198,13 +4376,13 @@
         <v>1</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>10</v>
@@ -4222,16 +4400,16 @@
         <v>10</v>
       </c>
       <c r="AC8" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AD8" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="AG8" s="4" t="s">
         <v>10</v>
@@ -4245,10 +4423,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>0</v>
@@ -4260,31 +4438,31 @@
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>1</v>
@@ -4296,16 +4474,16 @@
         <v>1</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>10</v>
@@ -4323,16 +4501,16 @@
         <v>10</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="AG9" s="2" t="s">
         <v>10</v>
@@ -4361,7 +4539,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>0</v>
@@ -4370,13 +4548,13 @@
         <v>115</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>117</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>117</v>
@@ -4391,34 +4569,34 @@
         <v>1</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>3</v>
@@ -4439,104 +4617,104 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="56" customFormat="1">
-      <c r="A11" s="55" t="s">
+    <row r="11" spans="1:33" s="5" customFormat="1">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="55" t="s">
+      <c r="E11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="55" t="s">
-        <v>306</v>
-      </c>
-      <c r="I11" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="55" t="s">
+      <c r="G11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K11" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="L11" s="55" t="s">
+      <c r="K11" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M11" s="55" t="s">
+      <c r="M11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N11" s="55" t="s">
+      <c r="N11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O11" s="55" t="s">
+      <c r="O11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="P11" s="55" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q11" s="55" t="s">
+      <c r="P11" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="55" t="s">
-        <v>287</v>
-      </c>
-      <c r="S11" s="55" t="s">
+      <c r="R11" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="T11" s="55" t="s">
+      <c r="T11" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="X11" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="U11" s="55" t="s">
-        <v>289</v>
-      </c>
-      <c r="V11" s="55" t="s">
-        <v>289</v>
-      </c>
-      <c r="W11" s="55" t="s">
-        <v>289</v>
-      </c>
-      <c r="X11" s="55" t="s">
-        <v>308</v>
-      </c>
-      <c r="Y11" s="55" t="s">
-        <v>309</v>
-      </c>
-      <c r="Z11" s="55" t="s">
+      <c r="Y11" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA11" s="55" t="s">
-        <v>310</v>
-      </c>
-      <c r="AB11" s="55" t="s">
+      <c r="AA11" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="AB11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AC11" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD11" s="55" t="s">
-        <v>307</v>
-      </c>
-      <c r="AE11" s="55" t="s">
+      <c r="AC11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF11" s="55" t="s">
+      <c r="AF11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AG11" s="55" t="s">
+      <c r="AG11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4548,10 +4726,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>0</v>
@@ -4563,31 +4741,31 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>1</v>
@@ -4599,16 +4777,16 @@
         <v>1</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>10</v>
@@ -4629,13 +4807,13 @@
         <v>10</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>10</v>
@@ -4649,10 +4827,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>0</v>
@@ -4664,37 +4842,37 @@
         <v>3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>138</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>138</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>1</v>
@@ -4703,25 +4881,25 @@
         <v>3</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AB13" s="2" t="s">
         <v>3</v>
@@ -4730,13 +4908,13 @@
         <v>10</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AG13" s="2" t="s">
         <v>10</v>
@@ -4750,10 +4928,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>0</v>
@@ -4765,31 +4943,31 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>1</v>
@@ -4804,13 +4982,13 @@
         <v>0</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>10</v>
@@ -4828,16 +5006,16 @@
         <v>10</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="AG14" s="2" t="s">
         <v>10</v>
@@ -4851,10 +5029,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>0</v>
@@ -4866,31 +5044,31 @@
         <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L15" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>1</v>
@@ -4902,16 +5080,16 @@
         <v>1</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>10</v>
@@ -4932,13 +5110,13 @@
         <v>10</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="AG15" s="2" t="s">
         <v>10</v>
@@ -4952,10 +5130,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>0</v>
@@ -4967,31 +5145,31 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>1</v>
@@ -5006,13 +5184,13 @@
         <v>0</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>10</v>
@@ -5030,16 +5208,16 @@
         <v>10</v>
       </c>
       <c r="AC16" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="AG16" s="2" t="s">
         <v>10</v>
@@ -5053,10 +5231,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>0</v>
@@ -5068,31 +5246,31 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>1</v>
@@ -5107,25 +5285,25 @@
         <v>0</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AB17" s="2" t="s">
         <v>3</v>
@@ -5134,408 +5312,408 @@
         <v>10</v>
       </c>
       <c r="AD17" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="15" customHeight="1">
+      <c r="C20" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="54" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z20" s="54"/>
+      <c r="AA20" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="AB20" s="54"/>
+      <c r="AC20" s="35" t="s">
+        <v>374</v>
+      </c>
+      <c r="AD20" s="35"/>
+    </row>
+    <row r="21" spans="1:34" ht="15" customHeight="1">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="54"/>
+      <c r="AA21" s="54"/>
+      <c r="AB21" s="54"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
+    </row>
+    <row r="22" spans="1:34">
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="54"/>
+      <c r="AA22" s="54"/>
+      <c r="AB22" s="54"/>
+      <c r="AC22" s="35"/>
+      <c r="AD22" s="35"/>
+    </row>
+    <row r="23" spans="1:34" ht="11.25" customHeight="1">
+      <c r="A23" s="52" t="s">
+        <v>347</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="I23" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="J23" s="34" t="s">
         <v>352</v>
       </c>
-      <c r="AF17" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" ht="15" customHeight="1">
-      <c r="C20" s="33" t="s">
-        <v>385</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="59" t="s">
-        <v>386</v>
-      </c>
-      <c r="Z20" s="59"/>
-      <c r="AA20" s="59" t="s">
-        <v>387</v>
-      </c>
-      <c r="AB20" s="59"/>
-      <c r="AC20" s="33" t="s">
-        <v>389</v>
-      </c>
-      <c r="AD20" s="33"/>
-    </row>
-    <row r="21" spans="1:34" ht="15" customHeight="1">
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="33"/>
-      <c r="Y21" s="59"/>
-      <c r="Z21" s="59"/>
-      <c r="AA21" s="59"/>
-      <c r="AB21" s="59"/>
-      <c r="AC21" s="33"/>
-      <c r="AD21" s="33"/>
-    </row>
-    <row r="22" spans="1:34">
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="33"/>
-      <c r="Y22" s="59"/>
-      <c r="Z22" s="59"/>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="33"/>
-      <c r="AD22" s="33"/>
-    </row>
-    <row r="23" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A23" s="46" t="s">
+      <c r="K23" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="L23" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="M23" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" s="32" t="s">
+      <c r="N23" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="O23" s="50" t="s">
+        <v>471</v>
+      </c>
+      <c r="P23" s="47" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q23" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="R23" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S23" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="T23" s="31" t="s">
+        <v>362</v>
+      </c>
+      <c r="U23" s="55" t="s">
+        <v>364</v>
+      </c>
+      <c r="V23" s="50" t="s">
+        <v>473</v>
+      </c>
+      <c r="W23" s="53" t="s">
+        <v>475</v>
+      </c>
+      <c r="X23" s="50" t="s">
+        <v>474</v>
+      </c>
+      <c r="Y23" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="Z23" s="34" t="s">
+        <v>366</v>
+      </c>
+      <c r="AA23" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="AB23" s="34" t="s">
+        <v>368</v>
+      </c>
+      <c r="AC23" s="34" t="s">
         <v>356</v>
       </c>
-      <c r="E23" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="F23" s="32" t="s">
+      <c r="AD23" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="G23" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="J23" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>362</v>
-      </c>
-      <c r="L23" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="M23" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="N23" s="48" t="s">
-        <v>364</v>
-      </c>
-      <c r="O23" s="45" t="s">
-        <v>365</v>
-      </c>
-      <c r="P23" s="49" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q23" s="32" t="s">
+      <c r="AE23" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF23" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG23" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="R23" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="S23" s="29" t="s">
-        <v>372</v>
-      </c>
-      <c r="T23" s="29" t="s">
-        <v>374</v>
-      </c>
-      <c r="U23" s="52" t="s">
-        <v>376</v>
-      </c>
-      <c r="V23" s="45" t="s">
-        <v>382</v>
-      </c>
-      <c r="W23" s="58" t="s">
-        <v>383</v>
-      </c>
-      <c r="X23" s="45" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y23" s="32" t="s">
-        <v>378</v>
-      </c>
-      <c r="Z23" s="32" t="s">
-        <v>379</v>
-      </c>
-      <c r="AA23" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="AB23" s="32" t="s">
-        <v>381</v>
-      </c>
-      <c r="AC23" s="32" t="s">
-        <v>367</v>
-      </c>
-      <c r="AD23" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="AE23" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="AF23" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="AG23" s="32" t="s">
-        <v>384</v>
-      </c>
       <c r="AH23" s="2"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="46"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="45"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="45"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="32"/>
-      <c r="AF24" s="32"/>
-      <c r="AG24" s="32"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="56"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="34"/>
+      <c r="AC24" s="34"/>
+      <c r="AD24" s="34"/>
+      <c r="AE24" s="34"/>
+      <c r="AF24" s="34"/>
+      <c r="AG24" s="34"/>
       <c r="AH24" s="2"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="46"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="53"/>
-      <c r="V25" s="45"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="45"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="32"/>
-      <c r="AA25" s="32"/>
-      <c r="AB25" s="32"/>
-      <c r="AC25" s="32"/>
-      <c r="AD25" s="32"/>
-      <c r="AE25" s="32"/>
-      <c r="AF25" s="32"/>
-      <c r="AG25" s="32"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="56"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34"/>
+      <c r="AE25" s="34"/>
+      <c r="AF25" s="34"/>
+      <c r="AG25" s="34"/>
       <c r="AH25" s="2"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="46"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="45"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="32"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="32"/>
-      <c r="AE26" s="32"/>
-      <c r="AF26" s="32"/>
-      <c r="AG26" s="32"/>
+      <c r="A26" s="52"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="48"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="56"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="53"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="34"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="34"/>
+      <c r="AC26" s="34"/>
+      <c r="AD26" s="34"/>
+      <c r="AE26" s="34"/>
+      <c r="AF26" s="34"/>
+      <c r="AG26" s="34"/>
       <c r="AH26" s="2"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="A27" s="46"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="54"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="58"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="32"/>
-      <c r="Z27" s="32"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="32"/>
-      <c r="AC27" s="32"/>
-      <c r="AD27" s="32"/>
-      <c r="AE27" s="32"/>
-      <c r="AF27" s="32"/>
-      <c r="AG27" s="32"/>
+      <c r="A27" s="52"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="34"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="34"/>
+      <c r="AE27" s="34"/>
+      <c r="AF27" s="34"/>
+      <c r="AG27" s="34"/>
       <c r="AH27" s="2"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="O28" s="45"/>
-      <c r="Q28" s="32"/>
-      <c r="V28" s="45"/>
-      <c r="W28" s="58"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="32"/>
+      <c r="O28" s="50"/>
+      <c r="Q28" s="34"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="34"/>
+      <c r="AB28" s="34"/>
+      <c r="AC28" s="34"/>
+      <c r="AD28" s="34"/>
     </row>
     <row r="29" spans="1:34">
-      <c r="G29" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="O29" s="45"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="S29" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="T29" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="V29" s="45"/>
-      <c r="W29" s="57"/>
-      <c r="X29" s="45"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
+      <c r="G29" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="O29" s="50"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="S29" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="T29" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="V29" s="50"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
     </row>
     <row r="30" spans="1:34" ht="236.25">
       <c r="G30" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R30" s="25" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="S30" s="25" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="T30" s="25" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="AC30" s="1"/>
       <c r="AD30" s="24"/>
@@ -5558,11 +5736,15 @@
     <mergeCell ref="Z23:Z29"/>
     <mergeCell ref="AA23:AA29"/>
     <mergeCell ref="AB23:AB29"/>
+    <mergeCell ref="J23:J27"/>
+    <mergeCell ref="K23:K27"/>
     <mergeCell ref="AC23:AC29"/>
     <mergeCell ref="AD23:AD29"/>
     <mergeCell ref="V23:V29"/>
     <mergeCell ref="Q23:Q29"/>
     <mergeCell ref="W23:W28"/>
+    <mergeCell ref="L23:L27"/>
+    <mergeCell ref="M23:M27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="P23:P27"/>
@@ -5577,10 +5759,6 @@
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="H23:H27"/>
     <mergeCell ref="I23:I27"/>
-    <mergeCell ref="J23:J27"/>
-    <mergeCell ref="K23:K27"/>
-    <mergeCell ref="L23:L27"/>
-    <mergeCell ref="M23:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5594,8 +5772,8 @@
   </sheetPr>
   <dimension ref="A2:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:J26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -5637,33 +5815,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21">
-      <c r="A3" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="43"/>
+      <c r="A3" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="45"/>
       <c r="C3" s="3" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
-        <v>420</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="A4" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
@@ -5677,7 +5855,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>95</v>
@@ -5686,22 +5864,22 @@
         <v>105</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -5709,31 +5887,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -5741,31 +5919,31 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -5773,31 +5951,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5805,31 +5983,31 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -5837,31 +6015,31 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5869,7 +6047,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>136</v>
@@ -5878,22 +6056,22 @@
         <v>141</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5901,149 +6079,1013 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A18" s="33" t="s">
-        <v>427</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="I18" s="60" t="s">
-        <v>428</v>
-      </c>
-      <c r="J18" s="60"/>
+      <c r="A18" s="35" t="s">
+        <v>412</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="I18" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="J18" s="58"/>
     </row>
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A21" s="32" t="s">
-        <v>418</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>419</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>421</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>422</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>423</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>424</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>425</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>429</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>430</v>
+      <c r="A21" s="34" t="s">
+        <v>403</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>406</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>407</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>409</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I18:J20"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="I21:I26"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="J21:J26"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="A18:G20"/>
-    <mergeCell ref="I21:I26"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="J21:J26"/>
-    <mergeCell ref="I18:J20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A2:AG22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25" style="2" customWidth="1"/>
+    <col min="24" max="24" width="26.85546875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="36.5703125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.5703125" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" ht="21">
+      <c r="A2" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="21">
+      <c r="A3" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" ht="21">
+      <c r="A4" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="1"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="52" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="52"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="52"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da Conferência LN - CAP
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CAP.xlsx
+++ b/Documentação/Planilhas/Conferencia_CAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="stg_cap_titulo_referencia" sheetId="94" r:id="rId5"/>
     <sheet name="stg_cap_titulo_reversao" sheetId="100" r:id="rId6"/>
     <sheet name="stg_cap_titulo_pgto" sheetId="98" r:id="rId7"/>
+    <sheet name="stg_cap_conciliacao_CAP_CAR" sheetId="101" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="539">
   <si>
     <t>1</t>
   </si>
@@ -1586,6 +1587,138 @@
   </si>
   <si>
     <t>Informar nos campos "Tipo Trans" e "Número do Documento" as informações desejadas e ir com a setinha de avanço até encontrar o registro, pois a view não tem o Cód Parceiro</t>
+  </si>
+  <si>
+    <t>dbo.stg_cap_conciliacao_CAP_CAR</t>
+  </si>
+  <si>
+    <t>CD_TP_TRANSACAO_BAIXA</t>
+  </si>
+  <si>
+    <t>NR_TRANSACAO_BAIXA</t>
+  </si>
+  <si>
+    <t>CD_TRANSACAO</t>
+  </si>
+  <si>
+    <t>NR_DOCUMENTO</t>
+  </si>
+  <si>
+    <t>VL_VALOR</t>
+  </si>
+  <si>
+    <t>CD_TP_TRANSACAO_REVERSAO</t>
+  </si>
+  <si>
+    <t>NR_TRANSACAO_REVERSAO</t>
+  </si>
+  <si>
+    <t>DT_BAIXA</t>
+  </si>
+  <si>
+    <t>ENC</t>
+  </si>
+  <si>
+    <t>PFA65</t>
+  </si>
+  <si>
+    <t>2014-06-14 00:00:00.000</t>
+  </si>
+  <si>
+    <t>RE4</t>
+  </si>
+  <si>
+    <t>RE415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pegar a informação da coluna "Parceiro de Negócios" </t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Doc. Baixa"</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Número do Documento"</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento do Doc.Baixa desejado. Pegar a informação da coluna "Tipo de Transação"</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento do Doc.Baixa desejado. Pegar a informação da coluna "No. Documento"</t>
+  </si>
+  <si>
+    <t>PFA206</t>
+  </si>
+  <si>
+    <t>2014-07-08 00:00:00.000</t>
+  </si>
+  <si>
+    <t>RE488</t>
+  </si>
+  <si>
+    <t>AFA4</t>
+  </si>
+  <si>
+    <t>2014-07-17 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2014-07-21 00:00:00.000</t>
+  </si>
+  <si>
+    <t>FAT</t>
+  </si>
+  <si>
+    <t>FAT198</t>
+  </si>
+  <si>
+    <t>FAT212</t>
+  </si>
+  <si>
+    <t>PKK</t>
+  </si>
+  <si>
+    <t>PKK28</t>
+  </si>
+  <si>
+    <t>RKL</t>
+  </si>
+  <si>
+    <t>RKL4</t>
+  </si>
+  <si>
+    <t>PKK29</t>
+  </si>
+  <si>
+    <t>2014-07-18 00:00:00.000</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento do Doc.Baixa desejado. Pegar a informação da coluna "Valor" [as transações de Pagamento virão negativas na view]</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento do Doc.Baixa desejado. Pegar a informação da coluna "Tipo de Transação de Reversão"</t>
+  </si>
+  <si>
+    <t>Pedir o detalhamento do Doc.Baixa desejado. Pegar a informação da coluna "Documento"</t>
+  </si>
+  <si>
+    <t>É a junção das informações das colunas "Tipo de Transação" com o "No. Documento"</t>
+  </si>
+  <si>
+    <t>Na Lupinha, pedir o filtro do CD_TIPO_TRANSACAO_BAIXA desejado. Pedir o detalhamento do  Nr Transação de Baixa desejado. Pegar a informação da coluna "Documento"</t>
+  </si>
+  <si>
+    <t>Na Lupinha, pedir o filtro do CD_TIPO_TRANSACAO_REVERSAO desejado. Pedir o detalhamento do  Nr Transação de Reversão desejado. Pegar a informação da coluna "Documento"</t>
+  </si>
+  <si>
+    <t>Sessão tfgld1504m000</t>
+  </si>
+  <si>
+    <t>znacrc217m000 e tfgld1504m000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   znacrc217m000 [Digitar o CD_PARCEIRO na caixa "Parceiro de Negócios" e pedir para filtrar os dados]</t>
+  </si>
+  <si>
+    <t>stg_cap_conciliacao_CAP_CAR</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1950,6 +2083,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1958,7 +2117,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2029,10 +2188,35 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2044,10 +2228,40 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2077,58 +2291,10 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2143,20 +2309,8 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2185,10 +2339,42 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2199,8 +2385,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFFFFCC"/>
+      <color rgb="FFCCECFF"/>
       <color rgb="FFFA7E7E"/>
-      <color rgb="FFCCECFF"/>
       <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
@@ -2537,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2588,10 +2774,16 @@
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="91" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="92"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="30" t="s">
+        <v>538</v>
+      </c>
+      <c r="C8" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2600,6 +2792,7 @@
     <hyperlink ref="B4" location="stg_cap_titulo_reembolso!A1" display="stg_cap_titulo_reembolso"/>
     <hyperlink ref="B5" location="stg_cap_titulo_referencia!A1" display="stg_cap_titulo_referencia"/>
     <hyperlink ref="B6" location="stg_cap_titulo_reversao!A1" display="stg_cap_titulo_reversao"/>
+    <hyperlink ref="B8" location="stg_cap_conciliacao_CAP_CAR!A1" display="stg_cap_conciliacao_CAP_CAR"/>
     <hyperlink ref="B7" location="stg_cap_titulo_pgto!A1" display="stg_cap_titulo_pgto"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2613,8 +2806,8 @@
   </sheetPr>
   <dimension ref="A2:AH30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F27"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2656,32 +2849,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="1"/>
       <c r="O4" s="12"/>
       <c r="P4" s="1"/>
@@ -3811,364 +4004,364 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1">
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="53" t="s">
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="33" t="s">
         <v>397</v>
       </c>
-      <c r="Z20" s="54"/>
-      <c r="AA20" s="53" t="s">
+      <c r="Z20" s="34"/>
+      <c r="AA20" s="33" t="s">
         <v>400</v>
       </c>
-      <c r="AB20" s="54"/>
-      <c r="AC20" s="34" t="s">
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="AD20" s="34"/>
+      <c r="AD20" s="32"/>
     </row>
     <row r="21" spans="1:34" ht="15" customHeight="1">
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="55"/>
-      <c r="AB21" s="56"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="34"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="32"/>
+      <c r="AD21" s="32"/>
     </row>
     <row r="22" spans="1:34">
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="57"/>
-      <c r="Z22" s="58"/>
-      <c r="AA22" s="57"/>
-      <c r="AB22" s="58"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="34"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="38"/>
+      <c r="AC22" s="32"/>
+      <c r="AD22" s="32"/>
     </row>
     <row r="23" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="53" t="s">
         <v>255</v>
       </c>
       <c r="B23" s="21"/>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="J23" s="33" t="s">
+      <c r="J23" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="K23" s="33" t="s">
+      <c r="K23" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="L23" s="33" t="s">
+      <c r="L23" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="33" t="s">
+      <c r="M23" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="N23" s="50" t="s">
+      <c r="N23" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="O23" s="49" t="s">
+      <c r="O23" s="45" t="s">
         <v>371</v>
       </c>
-      <c r="P23" s="46" t="s">
+      <c r="P23" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="Q23" s="33" t="s">
+      <c r="Q23" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="R23" s="33" t="s">
+      <c r="R23" s="31" t="s">
         <v>372</v>
       </c>
-      <c r="S23" s="30" t="s">
+      <c r="S23" s="39" t="s">
         <v>267</v>
       </c>
-      <c r="T23" s="30" t="s">
+      <c r="T23" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="U23" s="59" t="s">
+      <c r="U23" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="V23" s="49" t="s">
+      <c r="V23" s="45" t="s">
         <v>373</v>
       </c>
-      <c r="W23" s="52" t="s">
+      <c r="W23" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="X23" s="49" t="s">
+      <c r="X23" s="45" t="s">
         <v>374</v>
       </c>
-      <c r="Y23" s="33" t="s">
+      <c r="Y23" s="31" t="s">
         <v>398</v>
       </c>
-      <c r="Z23" s="33" t="s">
+      <c r="Z23" s="31" t="s">
         <v>399</v>
       </c>
-      <c r="AA23" s="33" t="s">
+      <c r="AA23" s="31" t="s">
         <v>401</v>
       </c>
-      <c r="AB23" s="33" t="s">
+      <c r="AB23" s="31" t="s">
         <v>402</v>
       </c>
-      <c r="AC23" s="33" t="s">
+      <c r="AC23" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="AD23" s="33" t="s">
+      <c r="AD23" s="31" t="s">
         <v>403</v>
       </c>
-      <c r="AE23" s="33" t="s">
+      <c r="AE23" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="AF23" s="33" t="s">
+      <c r="AF23" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="AG23" s="33" t="s">
+      <c r="AG23" s="31" t="s">
         <v>272</v>
       </c>
       <c r="AH23" s="2"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="51"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="21"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="49"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="49"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="33"/>
-      <c r="AD24" s="33"/>
-      <c r="AE24" s="33"/>
-      <c r="AF24" s="33"/>
-      <c r="AG24" s="33"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="47"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+      <c r="AG24" s="31"/>
       <c r="AH24" s="2"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="51"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="21"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="49"/>
-      <c r="W25" s="52"/>
-      <c r="X25" s="49"/>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
-      <c r="AA25" s="33"/>
-      <c r="AB25" s="33"/>
-      <c r="AC25" s="33"/>
-      <c r="AD25" s="33"/>
-      <c r="AE25" s="33"/>
-      <c r="AF25" s="33"/>
-      <c r="AG25" s="33"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="45"/>
+      <c r="W25" s="47"/>
+      <c r="X25" s="45"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+      <c r="AG25" s="31"/>
       <c r="AH25" s="2"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="51"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="60"/>
-      <c r="V26" s="49"/>
-      <c r="W26" s="52"/>
-      <c r="X26" s="49"/>
-      <c r="Y26" s="33"/>
-      <c r="Z26" s="33"/>
-      <c r="AA26" s="33"/>
-      <c r="AB26" s="33"/>
-      <c r="AC26" s="33"/>
-      <c r="AD26" s="33"/>
-      <c r="AE26" s="33"/>
-      <c r="AF26" s="33"/>
-      <c r="AG26" s="33"/>
+      <c r="A26" s="53"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="45"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="45"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="31"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="31"/>
+      <c r="AE26" s="31"/>
+      <c r="AF26" s="31"/>
+      <c r="AG26" s="31"/>
       <c r="AH26" s="2"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="A27" s="51"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="32"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="49"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="49"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="33"/>
-      <c r="AA27" s="33"/>
-      <c r="AB27" s="33"/>
-      <c r="AC27" s="33"/>
-      <c r="AD27" s="33"/>
-      <c r="AE27" s="33"/>
-      <c r="AF27" s="33"/>
-      <c r="AG27" s="33"/>
+      <c r="A27" s="53"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="45"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="31"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="31"/>
+      <c r="AE27" s="31"/>
+      <c r="AF27" s="31"/>
+      <c r="AG27" s="31"/>
       <c r="AH27" s="2"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="O28" s="49"/>
-      <c r="Q28" s="33"/>
-      <c r="V28" s="49"/>
-      <c r="W28" s="52"/>
-      <c r="X28" s="49"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="33"/>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="33"/>
-      <c r="AC28" s="33"/>
-      <c r="AD28" s="33"/>
+      <c r="O28" s="45"/>
+      <c r="Q28" s="31"/>
+      <c r="V28" s="45"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="45"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="31"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="31"/>
     </row>
     <row r="29" spans="1:34">
       <c r="G29" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="O29" s="49"/>
-      <c r="Q29" s="50"/>
+      <c r="O29" s="45"/>
+      <c r="Q29" s="46"/>
       <c r="R29" s="25" t="s">
         <v>85</v>
       </c>
@@ -4178,15 +4371,15 @@
       <c r="T29" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="V29" s="49"/>
+      <c r="V29" s="45"/>
       <c r="W29" s="26"/>
-      <c r="X29" s="49"/>
-      <c r="Y29" s="33"/>
-      <c r="Z29" s="33"/>
-      <c r="AA29" s="33"/>
-      <c r="AB29" s="33"/>
-      <c r="AC29" s="33"/>
-      <c r="AD29" s="33"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="31"/>
     </row>
     <row r="30" spans="1:34" ht="236.25">
       <c r="G30" s="24" t="s">
@@ -4206,6 +4399,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="P23:P27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="O23:O29"/>
+    <mergeCell ref="N23:N27"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="J23:J27"/>
+    <mergeCell ref="K23:K27"/>
+    <mergeCell ref="AC23:AC29"/>
+    <mergeCell ref="AD23:AD29"/>
+    <mergeCell ref="V23:V29"/>
+    <mergeCell ref="Q23:Q29"/>
+    <mergeCell ref="W23:W28"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="AB23:AB29"/>
     <mergeCell ref="L23:L27"/>
     <mergeCell ref="M23:M27"/>
     <mergeCell ref="AE23:AE27"/>
@@ -4222,29 +4438,6 @@
     <mergeCell ref="X23:X29"/>
     <mergeCell ref="Y23:Y29"/>
     <mergeCell ref="Z23:Z29"/>
-    <mergeCell ref="AC23:AC29"/>
-    <mergeCell ref="AD23:AD29"/>
-    <mergeCell ref="V23:V29"/>
-    <mergeCell ref="Q23:Q29"/>
-    <mergeCell ref="W23:W28"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="AB23:AB29"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="P23:P27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="O23:O29"/>
-    <mergeCell ref="N23:N27"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="J23:J27"/>
-    <mergeCell ref="K23:K27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4287,34 +4480,34 @@
       <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>72</v>
       </c>
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AC3" s="2"/>
     </row>
     <row r="4" spans="1:29" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="1"/>
       <c r="O4" s="12"/>
       <c r="AC4" s="2"/>
@@ -4944,26 +5137,26 @@
     <row r="20" spans="1:18" ht="11.25" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="15"/>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="54" t="s">
         <v>362</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="35" t="s">
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="54" t="s">
         <v>363</v>
       </c>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="28" t="s">
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="63" t="s">
         <v>365</v>
       </c>
-      <c r="Q20" s="34" t="s">
+      <c r="Q20" s="32" t="s">
         <v>95</v>
       </c>
       <c r="R20" s="2"/>
@@ -4971,136 +5164,136 @@
     <row r="21" spans="1:18" ht="11.25" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="34"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="32"/>
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" ht="11.25" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="17"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="34"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="32"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H23" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="L23" s="30" t="s">
+      <c r="L23" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="N23" s="30" t="s">
+      <c r="N23" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="O23" s="30" t="s">
+      <c r="O23" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="P23" s="30" t="s">
+      <c r="P23" s="39" t="s">
         <v>366</v>
       </c>
-      <c r="Q23" s="30" t="s">
+      <c r="Q23" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="R23" s="33" t="s">
+      <c r="R23" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="31"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="33"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="31"/>
     </row>
     <row r="27" spans="1:18">
       <c r="K27" s="18" t="s">
@@ -5123,11 +5316,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="P20:P22"/>
+    <mergeCell ref="P23:P25"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="Q20:Q22"/>
+    <mergeCell ref="Q23:Q25"/>
     <mergeCell ref="N23:N25"/>
     <mergeCell ref="G20:O22"/>
     <mergeCell ref="A23:A25"/>
@@ -5142,12 +5336,11 @@
     <mergeCell ref="I23:I25"/>
     <mergeCell ref="J23:J25"/>
     <mergeCell ref="K23:K25"/>
-    <mergeCell ref="P20:P22"/>
-    <mergeCell ref="P23:P25"/>
-    <mergeCell ref="O23:O25"/>
-    <mergeCell ref="R23:R25"/>
-    <mergeCell ref="Q20:Q22"/>
-    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="M23:M25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5162,7 +5355,7 @@
   </sheetPr>
   <dimension ref="A2:AG29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -5205,33 +5398,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="12"/>
       <c r="J4" s="12"/>
     </row>
@@ -5497,126 +5690,126 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="65" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="68" t="s">
         <v>313</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="62" t="s">
+      <c r="I18" s="68"/>
+      <c r="J18" s="65" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="63"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="66"/>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="64"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="67"/>
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="31" t="s">
         <v>305</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="I21" s="50" t="s">
+      <c r="I21" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="J21" s="49" t="s">
+      <c r="J21" s="45" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="49"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="45"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="49"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="H24" s="33"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="49"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="H25" s="33"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="49"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="45"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="H26" s="33"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="49"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="45"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="J27" s="49"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="J28" s="49"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="J29" s="49"/>
+      <c r="J29" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5665,20 +5858,20 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>148</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>153</v>
       </c>
@@ -5872,60 +6065,60 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="28" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="63" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="28"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="63"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="28"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="63"/>
     </row>
     <row r="22" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="39" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5951,7 +6144,7 @@
   </sheetPr>
   <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -5973,46 +6166,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="69" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
     </row>
     <row r="5" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
@@ -6433,87 +6626,89 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="31" t="s">
         <v>487</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="31" t="s">
         <v>477</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="31" t="s">
         <v>478</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="31" t="s">
         <v>479</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="31" t="s">
         <v>480</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="31" t="s">
         <v>481</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="31" t="s">
         <v>482</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="31" t="s">
         <v>483</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="31" t="s">
         <v>484</v>
       </c>
-      <c r="K21" s="33" t="s">
+      <c r="K21" s="31" t="s">
         <v>485</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="L21" s="31" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="K21:K24"/>
     <mergeCell ref="L21:L24"/>
     <mergeCell ref="A4:I5"/>
@@ -6527,8 +6722,6 @@
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="C21:C24"/>
     <mergeCell ref="D21:D24"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6583,32 +6776,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="21">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="3" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="21">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="3" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="1"/>
       <c r="L4" s="1"/>
       <c r="P4" s="1"/>
@@ -7397,38 +7590,38 @@
       </c>
     </row>
     <row r="20" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="54" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="71" t="s">
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="70" t="s">
         <v>409</v>
       </c>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="66" t="s">
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="81" t="s">
         <v>412</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="32" t="s">
         <v>413</v>
       </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="67" t="s">
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="79" t="s">
         <v>422</v>
       </c>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="32" t="s">
         <v>425</v>
       </c>
-      <c r="U20" s="34" t="s">
+      <c r="U20" s="32" t="s">
         <v>428</v>
       </c>
       <c r="AH20" s="2"/>
@@ -7436,120 +7629,120 @@
       <c r="AJ20" s="2"/>
     </row>
     <row r="21" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="68"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
     </row>
     <row r="22" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="68"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
     </row>
     <row r="23" spans="1:36" ht="11.25" customHeight="1">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="31" t="s">
         <v>408</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="31" t="s">
         <v>407</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="39" t="s">
         <v>429</v>
       </c>
-      <c r="K23" s="61" t="s">
+      <c r="K23" s="44" t="s">
         <v>410</v>
       </c>
-      <c r="L23" s="33" t="s">
+      <c r="L23" s="31" t="s">
         <v>414</v>
       </c>
-      <c r="M23" s="33" t="s">
+      <c r="M23" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="N23" s="33" t="s">
+      <c r="N23" s="31" t="s">
         <v>416</v>
       </c>
-      <c r="O23" s="33" t="s">
+      <c r="O23" s="31" t="s">
         <v>417</v>
       </c>
-      <c r="P23" s="33" t="s">
+      <c r="P23" s="31" t="s">
         <v>418</v>
       </c>
-      <c r="Q23" s="33" t="s">
+      <c r="Q23" s="31" t="s">
         <v>419</v>
       </c>
-      <c r="R23" s="50" t="s">
+      <c r="R23" s="46" t="s">
         <v>420</v>
       </c>
-      <c r="S23" s="33" t="s">
+      <c r="S23" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="T23" s="33" t="s">
+      <c r="T23" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="U23" s="33" t="s">
+      <c r="U23" s="31" t="s">
         <v>426</v>
       </c>
-      <c r="V23" s="49" t="s">
+      <c r="V23" s="45" t="s">
         <v>430</v>
       </c>
       <c r="AH23" s="2"/>
@@ -7557,144 +7750,160 @@
       <c r="AJ23" s="2"/>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="49"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="45"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="49"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="45"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="33"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="33"/>
-      <c r="V26" s="49"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="45"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="2"/>
     </row>
     <row r="27" spans="1:36">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="49"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="45"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="2"/>
     </row>
     <row r="28" spans="1:36">
-      <c r="R28" s="69"/>
-      <c r="T28" s="69"/>
-      <c r="V28" s="49"/>
+      <c r="R28" s="28"/>
+      <c r="T28" s="28"/>
+      <c r="V28" s="45"/>
     </row>
     <row r="29" spans="1:36">
       <c r="K29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="R29" s="69"/>
+      <c r="R29" s="28"/>
       <c r="T29" s="27" t="s">
         <v>85</v>
       </c>
       <c r="U29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="V29" s="49"/>
+      <c r="V29" s="45"/>
     </row>
     <row r="30" spans="1:36" ht="191.25">
       <c r="K30" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="T30" s="70" t="s">
+      <c r="T30" s="29" t="s">
         <v>424</v>
       </c>
-      <c r="U30" s="70" t="s">
+      <c r="U30" s="29" t="s">
         <v>427</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="R23:R27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="O23:O27"/>
+    <mergeCell ref="P23:P27"/>
+    <mergeCell ref="Q23:Q27"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="B20:D22"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="E23:E27"/>
     <mergeCell ref="V23:V29"/>
     <mergeCell ref="U20:U22"/>
     <mergeCell ref="U23:U27"/>
@@ -7704,31 +7913,696 @@
     <mergeCell ref="T20:T22"/>
     <mergeCell ref="T23:T27"/>
     <mergeCell ref="S23:S27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="F23:F27"/>
     <mergeCell ref="L20:R22"/>
     <mergeCell ref="M23:M27"/>
     <mergeCell ref="N23:N27"/>
     <mergeCell ref="K23:K27"/>
-    <mergeCell ref="B20:D22"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
     <mergeCell ref="K20:K22"/>
     <mergeCell ref="L23:L27"/>
     <mergeCell ref="I23:I27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="P23:P27"/>
-    <mergeCell ref="Q23:Q27"/>
-    <mergeCell ref="R23:R27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A2:AG27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" style="82" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="82" customWidth="1"/>
+    <col min="3" max="3" width="21" style="82" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="82" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="82" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="82" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="82" customWidth="1"/>
+    <col min="11" max="11" width="24" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="82"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" s="1" customFormat="1" ht="21">
+      <c r="A2" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" s="1" customFormat="1" ht="21">
+      <c r="A3" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>496</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>497</v>
+      </c>
+      <c r="D7" s="83" t="s">
+        <v>498</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>499</v>
+      </c>
+      <c r="F7" s="83" t="s">
+        <v>500</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H7" s="83" t="s">
+        <v>502</v>
+      </c>
+      <c r="I7" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="83" t="s">
+        <v>503</v>
+      </c>
+      <c r="K7" s="83" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C8" s="84">
+        <v>1</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>507</v>
+      </c>
+      <c r="E8" s="84">
+        <v>15</v>
+      </c>
+      <c r="F8" s="85">
+        <v>50000000</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" s="84">
+        <v>0</v>
+      </c>
+      <c r="I8" s="84" t="s">
+        <v>508</v>
+      </c>
+      <c r="J8" s="84" t="s">
+        <v>506</v>
+      </c>
+      <c r="K8" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="84"/>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C9" s="84">
+        <v>1</v>
+      </c>
+      <c r="D9" s="84" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="84">
+        <v>65</v>
+      </c>
+      <c r="F9" s="85">
+        <v>-50000000</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="84">
+        <v>0</v>
+      </c>
+      <c r="I9" s="84" t="s">
+        <v>505</v>
+      </c>
+      <c r="J9" s="84" t="s">
+        <v>506</v>
+      </c>
+      <c r="K9" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="84"/>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C10" s="84">
+        <v>21</v>
+      </c>
+      <c r="D10" s="84" t="s">
+        <v>225</v>
+      </c>
+      <c r="E10" s="84">
+        <v>206</v>
+      </c>
+      <c r="F10" s="85">
+        <v>-10000000</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H10" s="84">
+        <v>22</v>
+      </c>
+      <c r="I10" s="84" t="s">
+        <v>514</v>
+      </c>
+      <c r="J10" s="84" t="s">
+        <v>515</v>
+      </c>
+      <c r="K10" s="84" t="s">
+        <v>515</v>
+      </c>
+      <c r="L10" s="84"/>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C11" s="84">
+        <v>21</v>
+      </c>
+      <c r="D11" s="84" t="s">
+        <v>507</v>
+      </c>
+      <c r="E11" s="84">
+        <v>88</v>
+      </c>
+      <c r="F11" s="85">
+        <v>10000000</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H11" s="84">
+        <v>22</v>
+      </c>
+      <c r="I11" s="84" t="s">
+        <v>516</v>
+      </c>
+      <c r="J11" s="84" t="s">
+        <v>515</v>
+      </c>
+      <c r="K11" s="84" t="s">
+        <v>515</v>
+      </c>
+      <c r="L11" s="84"/>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12" s="84">
+        <v>26</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="84">
+        <v>4</v>
+      </c>
+      <c r="F12" s="85">
+        <v>-11000000</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H12" s="84">
+        <v>42</v>
+      </c>
+      <c r="I12" s="84" t="s">
+        <v>517</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="K12" s="84" t="s">
+        <v>519</v>
+      </c>
+      <c r="L12" s="84"/>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C13" s="84">
+        <v>26</v>
+      </c>
+      <c r="D13" s="84" t="s">
+        <v>520</v>
+      </c>
+      <c r="E13" s="84">
+        <v>198</v>
+      </c>
+      <c r="F13" s="85">
+        <v>10000000</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H13" s="84">
+        <v>42</v>
+      </c>
+      <c r="I13" s="84" t="s">
+        <v>521</v>
+      </c>
+      <c r="J13" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="K13" s="84" t="s">
+        <v>519</v>
+      </c>
+      <c r="L13" s="84"/>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" s="84">
+        <v>26</v>
+      </c>
+      <c r="D14" s="84" t="s">
+        <v>520</v>
+      </c>
+      <c r="E14" s="84">
+        <v>212</v>
+      </c>
+      <c r="F14" s="85">
+        <v>1000000</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H14" s="84">
+        <v>42</v>
+      </c>
+      <c r="I14" s="84" t="s">
+        <v>522</v>
+      </c>
+      <c r="J14" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="K14" s="84" t="s">
+        <v>519</v>
+      </c>
+      <c r="L14" s="84"/>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C15" s="84">
+        <v>37</v>
+      </c>
+      <c r="D15" s="84" t="s">
+        <v>523</v>
+      </c>
+      <c r="E15" s="84">
+        <v>28</v>
+      </c>
+      <c r="F15" s="85">
+        <v>-300000000</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H15" s="84">
+        <v>0</v>
+      </c>
+      <c r="I15" s="84" t="s">
+        <v>524</v>
+      </c>
+      <c r="J15" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="K15" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="84"/>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C16" s="84">
+        <v>37</v>
+      </c>
+      <c r="D16" s="84" t="s">
+        <v>525</v>
+      </c>
+      <c r="E16" s="84">
+        <v>4</v>
+      </c>
+      <c r="F16" s="85">
+        <v>300000000</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H16" s="84">
+        <v>0</v>
+      </c>
+      <c r="I16" s="84" t="s">
+        <v>526</v>
+      </c>
+      <c r="J16" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="K16" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="84"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="84" t="s">
+        <v>504</v>
+      </c>
+      <c r="C17" s="84">
+        <v>40</v>
+      </c>
+      <c r="D17" s="84" t="s">
+        <v>523</v>
+      </c>
+      <c r="E17" s="84">
+        <v>29</v>
+      </c>
+      <c r="F17" s="85">
+        <v>-300000000</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H17" s="84">
+        <v>41</v>
+      </c>
+      <c r="I17" s="84" t="s">
+        <v>527</v>
+      </c>
+      <c r="J17" s="84" t="s">
+        <v>528</v>
+      </c>
+      <c r="K17" s="84" t="s">
+        <v>519</v>
+      </c>
+      <c r="L17" s="84"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="86"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="84"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="89" t="s">
+        <v>537</v>
+      </c>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="90" t="s">
+        <v>535</v>
+      </c>
+      <c r="K19" s="90"/>
+      <c r="L19" s="84"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="89"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="89"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="89"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+    </row>
+    <row r="22" spans="1:12" ht="11.25" customHeight="1">
+      <c r="A22" s="87" t="s">
+        <v>509</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>510</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>511</v>
+      </c>
+      <c r="D22" s="87" t="s">
+        <v>512</v>
+      </c>
+      <c r="E22" s="87" t="s">
+        <v>513</v>
+      </c>
+      <c r="F22" s="87" t="s">
+        <v>532</v>
+      </c>
+      <c r="G22" s="87" t="s">
+        <v>529</v>
+      </c>
+      <c r="H22" s="87" t="s">
+        <v>530</v>
+      </c>
+      <c r="I22" s="87" t="s">
+        <v>531</v>
+      </c>
+      <c r="J22" s="87" t="s">
+        <v>533</v>
+      </c>
+      <c r="K22" s="87" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="87"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="87"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="87"/>
+      <c r="K24" s="87"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="87"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="87"/>
+      <c r="K25" s="87"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="87"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="87"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="A19:I21"/>
+    <mergeCell ref="J19:K21"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="G22:G27"/>
+    <mergeCell ref="H22:H27"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização Mapeamento de Conferência LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_CAP.xlsx
+++ b/Documentação/Planilhas/Conferencia_CAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="539">
   <si>
     <t>1</t>
   </si>
@@ -2117,7 +2117,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2168,9 +2168,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2195,7 +2192,52 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2237,31 +2279,10 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2289,12 +2310,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2348,24 +2363,8 @@
     <xf numFmtId="49" fontId="9" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2373,8 +2372,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2725,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2774,13 +2771,13 @@
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="36" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="92"/>
+      <c r="C7" s="37"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>538</v>
       </c>
       <c r="C8" s="11"/>
@@ -2806,8 +2803,8 @@
   </sheetPr>
   <dimension ref="A2:AH30"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C27"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2849,32 +2846,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>369</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="1"/>
       <c r="O4" s="12"/>
       <c r="P4" s="1"/>
@@ -4004,401 +4001,429 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1">
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="33" t="s">
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="33" t="s">
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="32" t="s">
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="AD20" s="32"/>
+      <c r="AD20" s="48"/>
     </row>
     <row r="21" spans="1:34" ht="15" customHeight="1">
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="32"/>
-      <c r="AD21" s="32"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="52"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="52"/>
+      <c r="AC21" s="48"/>
+      <c r="AD21" s="48"/>
     </row>
     <row r="22" spans="1:34">
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="38"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="38"/>
-      <c r="AC22" s="32"/>
-      <c r="AD22" s="32"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="53"/>
+      <c r="Z22" s="54"/>
+      <c r="AA22" s="53"/>
+      <c r="AB22" s="54"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
     </row>
     <row r="23" spans="1:34" ht="11.25" customHeight="1">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="46" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="31" t="s">
+      <c r="B23" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="L23" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="N23" s="46" t="s">
+      <c r="N23" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="O23" s="45" t="s">
+      <c r="O23" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="P23" s="49" t="s">
+      <c r="P23" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="Q23" s="31" t="s">
+      <c r="Q23" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="R23" s="31" t="s">
+      <c r="R23" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="S23" s="39" t="s">
+      <c r="S23" s="55" t="s">
         <v>267</v>
       </c>
-      <c r="T23" s="39" t="s">
+      <c r="T23" s="55" t="s">
         <v>269</v>
       </c>
-      <c r="U23" s="42" t="s">
+      <c r="U23" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="V23" s="45" t="s">
+      <c r="V23" s="43" t="s">
         <v>373</v>
       </c>
       <c r="W23" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="X23" s="45" t="s">
+      <c r="X23" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="Y23" s="31" t="s">
+      <c r="Y23" s="42" t="s">
         <v>398</v>
       </c>
-      <c r="Z23" s="31" t="s">
+      <c r="Z23" s="42" t="s">
         <v>399</v>
       </c>
-      <c r="AA23" s="31" t="s">
+      <c r="AA23" s="42" t="s">
         <v>401</v>
       </c>
-      <c r="AB23" s="31" t="s">
+      <c r="AB23" s="42" t="s">
         <v>402</v>
       </c>
-      <c r="AC23" s="31" t="s">
+      <c r="AC23" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="AD23" s="31" t="s">
+      <c r="AD23" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="AE23" s="31" t="s">
+      <c r="AE23" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="AF23" s="31" t="s">
+      <c r="AF23" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="AG23" s="31" t="s">
+      <c r="AG23" s="42" t="s">
         <v>272</v>
       </c>
       <c r="AH23" s="2"/>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="53"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="45"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="56"/>
+      <c r="T24" s="56"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="43"/>
       <c r="W24" s="47"/>
-      <c r="X24" s="45"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-      <c r="AG24" s="31"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42"/>
+      <c r="AG24" s="42"/>
       <c r="AH24" s="2"/>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="53"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="45"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="43"/>
       <c r="W25" s="47"/>
-      <c r="X25" s="45"/>
-      <c r="Y25" s="31"/>
-      <c r="Z25" s="31"/>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="31"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="31"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="42"/>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="42"/>
+      <c r="AE25" s="42"/>
+      <c r="AF25" s="42"/>
+      <c r="AG25" s="42"/>
       <c r="AH25" s="2"/>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="53"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="45"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="43"/>
       <c r="W26" s="47"/>
-      <c r="X26" s="45"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="42"/>
+      <c r="Z26" s="42"/>
+      <c r="AA26" s="42"/>
+      <c r="AB26" s="42"/>
+      <c r="AC26" s="42"/>
+      <c r="AD26" s="42"/>
+      <c r="AE26" s="42"/>
+      <c r="AF26" s="42"/>
+      <c r="AG26" s="42"/>
       <c r="AH26" s="2"/>
     </row>
     <row r="27" spans="1:34">
-      <c r="A27" s="53"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="45"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="43"/>
       <c r="W27" s="47"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="31"/>
-      <c r="Z27" s="31"/>
-      <c r="AA27" s="31"/>
-      <c r="AB27" s="31"/>
-      <c r="AC27" s="31"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="31"/>
-      <c r="AF27" s="31"/>
-      <c r="AG27" s="31"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="42"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="42"/>
+      <c r="AC27" s="42"/>
+      <c r="AD27" s="42"/>
+      <c r="AE27" s="42"/>
+      <c r="AF27" s="42"/>
+      <c r="AG27" s="42"/>
       <c r="AH27" s="2"/>
     </row>
     <row r="28" spans="1:34">
-      <c r="O28" s="45"/>
-      <c r="Q28" s="31"/>
-      <c r="V28" s="45"/>
+      <c r="O28" s="43"/>
+      <c r="Q28" s="42"/>
+      <c r="V28" s="43"/>
       <c r="W28" s="47"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="31"/>
-      <c r="Z28" s="31"/>
-      <c r="AA28" s="31"/>
-      <c r="AB28" s="31"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="31"/>
+      <c r="X28" s="43"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="42"/>
+      <c r="AA28" s="42"/>
+      <c r="AB28" s="42"/>
+      <c r="AC28" s="42"/>
+      <c r="AD28" s="42"/>
     </row>
     <row r="29" spans="1:34">
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="O29" s="45"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="25" t="s">
+      <c r="O29" s="43"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="S29" s="25" t="s">
+      <c r="S29" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="T29" s="25" t="s">
+      <c r="T29" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="V29" s="45"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="45"/>
-      <c r="Y29" s="31"/>
-      <c r="Z29" s="31"/>
-      <c r="AA29" s="31"/>
-      <c r="AB29" s="31"/>
-      <c r="AC29" s="31"/>
-      <c r="AD29" s="31"/>
+      <c r="V29" s="43"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="42"/>
+      <c r="Z29" s="42"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="42"/>
+      <c r="AC29" s="42"/>
+      <c r="AD29" s="42"/>
     </row>
     <row r="30" spans="1:34" ht="236.25">
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="R30" s="23" t="s">
+      <c r="R30" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="S30" s="23" t="s">
+      <c r="S30" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="T30" s="23" t="s">
+      <c r="T30" s="22" t="s">
         <v>270</v>
       </c>
       <c r="AC30" s="1"/>
-      <c r="AD30" s="22"/>
+      <c r="AD30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="40">
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="L23:L27"/>
+    <mergeCell ref="M23:M27"/>
+    <mergeCell ref="AE23:AE27"/>
+    <mergeCell ref="AG23:AG27"/>
+    <mergeCell ref="C20:X22"/>
+    <mergeCell ref="Y20:Z22"/>
+    <mergeCell ref="AA20:AB22"/>
+    <mergeCell ref="AC20:AD22"/>
+    <mergeCell ref="R23:R27"/>
+    <mergeCell ref="S23:S27"/>
+    <mergeCell ref="AF23:AF27"/>
+    <mergeCell ref="T23:T27"/>
+    <mergeCell ref="U23:U27"/>
+    <mergeCell ref="X23:X29"/>
+    <mergeCell ref="Y23:Y29"/>
+    <mergeCell ref="Z23:Z29"/>
+    <mergeCell ref="AC23:AC29"/>
+    <mergeCell ref="AD23:AD29"/>
+    <mergeCell ref="V23:V29"/>
+    <mergeCell ref="Q23:Q29"/>
+    <mergeCell ref="W23:W28"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="AB23:AB29"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="P23:P27"/>
@@ -4415,29 +4440,6 @@
     <mergeCell ref="I23:I27"/>
     <mergeCell ref="J23:J27"/>
     <mergeCell ref="K23:K27"/>
-    <mergeCell ref="AC23:AC29"/>
-    <mergeCell ref="AD23:AD29"/>
-    <mergeCell ref="V23:V29"/>
-    <mergeCell ref="Q23:Q29"/>
-    <mergeCell ref="W23:W28"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="AB23:AB29"/>
-    <mergeCell ref="L23:L27"/>
-    <mergeCell ref="M23:M27"/>
-    <mergeCell ref="AE23:AE27"/>
-    <mergeCell ref="AG23:AG27"/>
-    <mergeCell ref="C20:X22"/>
-    <mergeCell ref="Y20:Z22"/>
-    <mergeCell ref="AA20:AB22"/>
-    <mergeCell ref="AC20:AD22"/>
-    <mergeCell ref="R23:R27"/>
-    <mergeCell ref="S23:S27"/>
-    <mergeCell ref="AF23:AF27"/>
-    <mergeCell ref="T23:T27"/>
-    <mergeCell ref="U23:U27"/>
-    <mergeCell ref="X23:X29"/>
-    <mergeCell ref="Y23:Y29"/>
-    <mergeCell ref="Z23:Z29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4480,34 +4482,34 @@
       <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>72</v>
       </c>
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AC3" s="2"/>
     </row>
     <row r="4" spans="1:29" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>369</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="1"/>
       <c r="O4" s="12"/>
       <c r="AC4" s="2"/>
@@ -5137,26 +5139,26 @@
     <row r="20" spans="1:18" ht="11.25" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="15"/>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="63" t="s">
         <v>362</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="54" t="s">
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="63" t="s">
         <v>363</v>
       </c>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="63" t="s">
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="61" t="s">
         <v>365</v>
       </c>
-      <c r="Q20" s="32" t="s">
+      <c r="Q20" s="48" t="s">
         <v>95</v>
       </c>
       <c r="R20" s="2"/>
@@ -5164,136 +5166,136 @@
     <row r="21" spans="1:18" ht="11.25" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="32"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="48"/>
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" ht="11.25" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="17"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="32"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="48"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="39" t="s">
+      <c r="H23" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="39" t="s">
+      <c r="I23" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="K23" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="39" t="s">
+      <c r="M23" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="N23" s="39" t="s">
+      <c r="N23" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="O23" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="P23" s="39" t="s">
+      <c r="P23" s="55" t="s">
         <v>366</v>
       </c>
-      <c r="Q23" s="39" t="s">
+      <c r="Q23" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="R23" s="31" t="s">
+      <c r="R23" s="42" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="31"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="42"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="31"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="42"/>
     </row>
     <row r="27" spans="1:18">
       <c r="K27" s="18" t="s">
@@ -5307,21 +5309,20 @@
       <c r="K28" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="O28" s="23" t="s">
+      <c r="O28" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="P28" s="22"/>
+      <c r="P28" s="21"/>
       <c r="Q28" s="20"/>
-      <c r="R28" s="22"/>
+      <c r="R28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="P20:P22"/>
-    <mergeCell ref="P23:P25"/>
-    <mergeCell ref="O23:O25"/>
-    <mergeCell ref="R23:R25"/>
-    <mergeCell ref="Q20:Q22"/>
-    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="M23:M25"/>
     <mergeCell ref="N23:N25"/>
     <mergeCell ref="G20:O22"/>
     <mergeCell ref="A23:A25"/>
@@ -5336,11 +5337,12 @@
     <mergeCell ref="I23:I25"/>
     <mergeCell ref="J23:J25"/>
     <mergeCell ref="K23:K25"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="P20:P22"/>
+    <mergeCell ref="P23:P25"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="Q20:Q22"/>
+    <mergeCell ref="Q23:Q25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5398,33 +5400,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>306</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="H4" s="12"/>
       <c r="J4" s="12"/>
     </row>
@@ -5690,126 +5692,126 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="68" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="I18" s="68"/>
-      <c r="J18" s="65" t="s">
+      <c r="I18" s="75"/>
+      <c r="J18" s="72" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="66"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="73"/>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="67"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="74"/>
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="42" t="s">
         <v>310</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="42" t="s">
         <v>314</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="44" t="s">
         <v>315</v>
       </c>
-      <c r="J21" s="45" t="s">
+      <c r="J21" s="43" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="45"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="45"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="H24" s="31"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="45"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="43"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="H25" s="31"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="45"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="H26" s="31"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="45"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="J27" s="45"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="J28" s="45"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="J29" s="45"/>
+      <c r="J29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5858,20 +5860,20 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>148</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>153</v>
       </c>
@@ -6065,60 +6067,60 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="63" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="61" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="63"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="61"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="63"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="55" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6166,46 +6168,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="76" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
@@ -6626,84 +6628,84 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="42" t="s">
         <v>487</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="42" t="s">
         <v>478</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="42" t="s">
         <v>479</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="42" t="s">
         <v>480</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="42" t="s">
         <v>481</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="42" t="s">
         <v>482</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="J21" s="31" t="s">
+      <c r="J21" s="42" t="s">
         <v>484</v>
       </c>
-      <c r="K21" s="31" t="s">
+      <c r="K21" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="L21" s="31" t="s">
+      <c r="L21" s="42" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -6776,32 +6778,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="1"/>
       <c r="L4" s="1"/>
       <c r="P4" s="1"/>
@@ -7590,38 +7592,38 @@
       </c>
     </row>
     <row r="20" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="63" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="70" t="s">
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="77" t="s">
         <v>409</v>
       </c>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="81" t="s">
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="88" t="s">
         <v>412</v>
       </c>
-      <c r="L20" s="32" t="s">
+      <c r="L20" s="48" t="s">
         <v>413</v>
       </c>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="79" t="s">
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="86" t="s">
         <v>422</v>
       </c>
-      <c r="T20" s="32" t="s">
+      <c r="T20" s="48" t="s">
         <v>425</v>
       </c>
-      <c r="U20" s="32" t="s">
+      <c r="U20" s="48" t="s">
         <v>428</v>
       </c>
       <c r="AH20" s="2"/>
@@ -7629,120 +7631,120 @@
       <c r="AJ20" s="2"/>
     </row>
     <row r="21" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B21" s="57"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="80"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="87"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
     </row>
     <row r="22" spans="1:36" ht="11.25" customHeight="1">
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="80"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="87"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
     </row>
     <row r="23" spans="1:36" ht="11.25" customHeight="1">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="42" t="s">
         <v>408</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="42" t="s">
         <v>407</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="55" t="s">
         <v>429</v>
       </c>
-      <c r="K23" s="44" t="s">
+      <c r="K23" s="60" t="s">
         <v>410</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="L23" s="42" t="s">
         <v>414</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="42" t="s">
         <v>415</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="42" t="s">
         <v>416</v>
       </c>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="42" t="s">
         <v>417</v>
       </c>
-      <c r="P23" s="31" t="s">
+      <c r="P23" s="42" t="s">
         <v>418</v>
       </c>
-      <c r="Q23" s="31" t="s">
+      <c r="Q23" s="42" t="s">
         <v>419</v>
       </c>
-      <c r="R23" s="46" t="s">
+      <c r="R23" s="44" t="s">
         <v>420</v>
       </c>
-      <c r="S23" s="31" t="s">
+      <c r="S23" s="42" t="s">
         <v>421</v>
       </c>
-      <c r="T23" s="31" t="s">
+      <c r="T23" s="42" t="s">
         <v>423</v>
       </c>
-      <c r="U23" s="31" t="s">
+      <c r="U23" s="42" t="s">
         <v>426</v>
       </c>
-      <c r="V23" s="45" t="s">
+      <c r="V23" s="43" t="s">
         <v>430</v>
       </c>
       <c r="AH23" s="2"/>
@@ -7750,160 +7752,144 @@
       <c r="AJ23" s="2"/>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="45"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="43"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="31"/>
-      <c r="V25" s="45"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="43"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="45"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="43"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="2"/>
     </row>
     <row r="27" spans="1:36">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="45"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="43"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="2"/>
     </row>
     <row r="28" spans="1:36">
-      <c r="R28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="V28" s="45"/>
+      <c r="R28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="V28" s="43"/>
     </row>
     <row r="29" spans="1:36">
       <c r="K29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="R29" s="28"/>
-      <c r="T29" s="27" t="s">
+      <c r="R29" s="27"/>
+      <c r="T29" s="26" t="s">
         <v>85</v>
       </c>
       <c r="U29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="V29" s="45"/>
+      <c r="V29" s="43"/>
     </row>
     <row r="30" spans="1:36" ht="191.25">
       <c r="K30" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="T30" s="29" t="s">
+      <c r="T30" s="28" t="s">
         <v>424</v>
       </c>
-      <c r="U30" s="29" t="s">
+      <c r="U30" s="28" t="s">
         <v>427</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="R23:R27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="P23:P27"/>
-    <mergeCell ref="Q23:Q27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="B20:D22"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
     <mergeCell ref="V23:V29"/>
     <mergeCell ref="U20:U22"/>
     <mergeCell ref="U23:U27"/>
@@ -7920,6 +7906,22 @@
     <mergeCell ref="K20:K22"/>
     <mergeCell ref="L23:L27"/>
     <mergeCell ref="I23:I27"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="B20:D22"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="R23:R27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="O23:O27"/>
+    <mergeCell ref="P23:P27"/>
+    <mergeCell ref="Q23:Q27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7933,31 +7935,31 @@
   </sheetPr>
   <dimension ref="A2:AG27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="82" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="82" customWidth="1"/>
-    <col min="3" max="3" width="21" style="82" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="82" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="82" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="21" style="30" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="82" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="82" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="82" customWidth="1"/>
-    <col min="11" max="11" width="24" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="82"/>
+    <col min="8" max="8" width="22.5703125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="30" customWidth="1"/>
+    <col min="11" max="11" width="24" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:33" s="1" customFormat="1" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="3" t="s">
         <v>495</v>
       </c>
@@ -7993,10 +7995,10 @@
       <c r="AG2" s="2"/>
     </row>
     <row r="3" spans="1:33" s="1" customFormat="1" ht="21">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>536</v>
       </c>
@@ -8035,557 +8037,562 @@
       <c r="A7" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="31" t="s">
         <v>496</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="31" t="s">
         <v>497</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="31" t="s">
         <v>498</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="31" t="s">
         <v>499</v>
       </c>
-      <c r="F7" s="83" t="s">
+      <c r="F7" s="31" t="s">
         <v>500</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="31" t="s">
         <v>502</v>
       </c>
-      <c r="I7" s="83" t="s">
+      <c r="I7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="83" t="s">
+      <c r="J7" s="31" t="s">
         <v>503</v>
       </c>
-      <c r="K7" s="83" t="s">
+      <c r="K7" s="31" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:33">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C8" s="84">
+      <c r="C8" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="32" t="s">
         <v>507</v>
       </c>
-      <c r="E8" s="84">
+      <c r="E8" s="32">
         <v>15</v>
       </c>
-      <c r="F8" s="85">
+      <c r="F8" s="33">
         <v>50000000</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="84">
-        <v>0</v>
-      </c>
-      <c r="I8" s="84" t="s">
+      <c r="H8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>508</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="32" t="s">
         <v>506</v>
       </c>
-      <c r="K8" s="84" t="s">
+      <c r="K8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="84"/>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" spans="1:33">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C9" s="84">
+      <c r="C9" s="32">
         <v>1</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="E9" s="84">
+      <c r="E9" s="32">
         <v>65</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="33">
         <v>-50000000</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H9" s="84">
-        <v>0</v>
-      </c>
-      <c r="I9" s="84" t="s">
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32" t="s">
         <v>505</v>
       </c>
-      <c r="J9" s="84" t="s">
+      <c r="J9" s="32" t="s">
         <v>506</v>
       </c>
-      <c r="K9" s="84" t="s">
+      <c r="K9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="84"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:33">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C10" s="84">
+      <c r="C10" s="32">
         <v>21</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="E10" s="84">
+      <c r="E10" s="32">
         <v>206</v>
       </c>
-      <c r="F10" s="85">
+      <c r="F10" s="33">
         <v>-10000000</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H10" s="84">
+      <c r="H10" s="32">
         <v>22</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="32" t="s">
         <v>514</v>
       </c>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="32" t="s">
         <v>515</v>
       </c>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="32" t="s">
         <v>515</v>
       </c>
-      <c r="L10" s="84"/>
+      <c r="L10" s="32"/>
     </row>
     <row r="11" spans="1:33">
-      <c r="A11" s="88" t="s">
+      <c r="A11" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C11" s="84">
+      <c r="C11" s="32">
         <v>21</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="32" t="s">
         <v>507</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="32">
         <v>88</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="33">
         <v>10000000</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H11" s="84">
+      <c r="H11" s="32">
         <v>22</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="32" t="s">
         <v>516</v>
       </c>
-      <c r="J11" s="84" t="s">
+      <c r="J11" s="32" t="s">
         <v>515</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="32" t="s">
         <v>515</v>
       </c>
-      <c r="L11" s="84"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:33">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C12" s="84">
+      <c r="C12" s="32">
         <v>26</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="84">
+      <c r="E12" s="32">
         <v>4</v>
       </c>
-      <c r="F12" s="85">
+      <c r="F12" s="33">
         <v>-11000000</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H12" s="84">
+      <c r="H12" s="32">
         <v>42</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="J12" s="84" t="s">
+      <c r="J12" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="K12" s="84" t="s">
+      <c r="K12" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="L12" s="84"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="1:33">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C13" s="84">
+      <c r="C13" s="32">
         <v>26</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="32" t="s">
         <v>520</v>
       </c>
-      <c r="E13" s="84">
+      <c r="E13" s="32">
         <v>198</v>
       </c>
-      <c r="F13" s="85">
+      <c r="F13" s="33">
         <v>10000000</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H13" s="84">
+      <c r="H13" s="32">
         <v>42</v>
       </c>
-      <c r="I13" s="84" t="s">
+      <c r="I13" s="32" t="s">
         <v>521</v>
       </c>
-      <c r="J13" s="84" t="s">
+      <c r="J13" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="K13" s="84" t="s">
+      <c r="K13" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="L13" s="84"/>
+      <c r="L13" s="32"/>
     </row>
     <row r="14" spans="1:33">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C14" s="84">
+      <c r="C14" s="32">
         <v>26</v>
       </c>
-      <c r="D14" s="84" t="s">
+      <c r="D14" s="32" t="s">
         <v>520</v>
       </c>
-      <c r="E14" s="84">
+      <c r="E14" s="32">
         <v>212</v>
       </c>
-      <c r="F14" s="85">
+      <c r="F14" s="33">
         <v>1000000</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H14" s="84">
+      <c r="H14" s="32">
         <v>42</v>
       </c>
-      <c r="I14" s="84" t="s">
+      <c r="I14" s="32" t="s">
         <v>522</v>
       </c>
-      <c r="J14" s="84" t="s">
+      <c r="J14" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="K14" s="84" t="s">
+      <c r="K14" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="L14" s="84"/>
+      <c r="L14" s="32"/>
     </row>
     <row r="15" spans="1:33">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C15" s="84">
+      <c r="C15" s="32">
         <v>37</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="32" t="s">
         <v>523</v>
       </c>
-      <c r="E15" s="84">
+      <c r="E15" s="32">
         <v>28</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="33">
         <v>-300000000</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H15" s="84">
-        <v>0</v>
-      </c>
-      <c r="I15" s="84" t="s">
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32" t="s">
         <v>524</v>
       </c>
-      <c r="J15" s="84" t="s">
+      <c r="J15" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="K15" s="84" t="s">
+      <c r="K15" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="84"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" spans="1:33">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C16" s="84">
+      <c r="C16" s="32">
         <v>37</v>
       </c>
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="32" t="s">
         <v>525</v>
       </c>
-      <c r="E16" s="84">
+      <c r="E16" s="32">
         <v>4</v>
       </c>
-      <c r="F16" s="85">
+      <c r="F16" s="33">
         <v>300000000</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H16" s="84">
-        <v>0</v>
-      </c>
-      <c r="I16" s="84" t="s">
+      <c r="H16" s="32">
+        <v>0</v>
+      </c>
+      <c r="I16" s="32" t="s">
         <v>526</v>
       </c>
-      <c r="J16" s="84" t="s">
+      <c r="J16" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="K16" s="84" t="s">
+      <c r="K16" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="84"/>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="C17" s="84">
+      <c r="C17" s="32">
         <v>40</v>
       </c>
-      <c r="D17" s="84" t="s">
+      <c r="D17" s="32" t="s">
         <v>523</v>
       </c>
-      <c r="E17" s="84">
+      <c r="E17" s="32">
         <v>29</v>
       </c>
-      <c r="F17" s="85">
+      <c r="F17" s="33">
         <v>-300000000</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H17" s="84">
+      <c r="H17" s="32">
         <v>41</v>
       </c>
-      <c r="I17" s="84" t="s">
+      <c r="I17" s="32" t="s">
         <v>527</v>
       </c>
-      <c r="J17" s="84" t="s">
+      <c r="J17" s="32" t="s">
         <v>528</v>
       </c>
-      <c r="K17" s="84" t="s">
+      <c r="K17" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="L17" s="84"/>
+      <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="86"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="90" t="s">
         <v>537</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="90" t="s">
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="91" t="s">
         <v>535</v>
       </c>
-      <c r="K19" s="90"/>
-      <c r="L19" s="84"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="32"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="89"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
+      <c r="A20" s="90"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="90"/>
-      <c r="K21" s="90"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
     </row>
     <row r="22" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="89" t="s">
         <v>509</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="89" t="s">
         <v>510</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="89" t="s">
         <v>511</v>
       </c>
-      <c r="D22" s="87" t="s">
+      <c r="D22" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="E22" s="87" t="s">
+      <c r="E22" s="89" t="s">
         <v>513</v>
       </c>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="89" t="s">
         <v>532</v>
       </c>
-      <c r="G22" s="87" t="s">
+      <c r="G22" s="89" t="s">
         <v>529</v>
       </c>
-      <c r="H22" s="87" t="s">
+      <c r="H22" s="89" t="s">
         <v>530</v>
       </c>
-      <c r="I22" s="87" t="s">
+      <c r="I22" s="89" t="s">
         <v>531</v>
       </c>
-      <c r="J22" s="87" t="s">
+      <c r="J22" s="89" t="s">
         <v>533</v>
       </c>
-      <c r="K22" s="87" t="s">
+      <c r="K22" s="89" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="87"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
+      <c r="A23" s="89"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="87"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="87"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="87"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
     <mergeCell ref="K22:K27"/>
     <mergeCell ref="A19:I21"/>
     <mergeCell ref="J19:K21"/>
@@ -8595,11 +8602,6 @@
     <mergeCell ref="I22:I27"/>
     <mergeCell ref="F22:F27"/>
     <mergeCell ref="J22:J27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="C22:C27"/>
     <mergeCell ref="D22:D27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>